<commit_message>
Historia de usuario - doc
</commit_message>
<xml_diff>
--- a/docs/Historias de USUARIO.xlsx
+++ b/docs/Historias de USUARIO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jp\Desktop\Proyecto Final y Test Empresas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jp\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FB09AC-C3A7-4023-A69C-22F0A072ECF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59BB8E9-7CFA-4402-BC17-858FF4DA1D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C8424CB0-D5B6-4AE2-9447-D320E95AD064}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>HU - 1</t>
   </si>
@@ -115,15 +115,9 @@
     <t>HU RELACIONADAS A LOS PEDIDOS Y PRODUCTOS</t>
   </si>
   <si>
-    <t xml:space="preserve">HU - 9 Yo como usuario registrado quiero revisar el DETALLE DEL PEDIDO. </t>
-  </si>
-  <si>
     <t xml:space="preserve">HU - 8 Yo como usuario registrado, quiero ir agregando estos productos a un PEDIDO. </t>
   </si>
   <si>
-    <t xml:space="preserve">HU - 10 Yo como usuario registrado, quiero ver el resumen de mi medido e ingresar la orden de compra/solicitud. </t>
-  </si>
-  <si>
     <t>HU - 2  Yo como usuario registrado, quiero ver los productos de la pagina con mi cuenta registrada.</t>
   </si>
   <si>
@@ -136,7 +130,10 @@
     <t>HU - 7  Yo como usuario registrado quiero ver la informacion del producto, precio y descripcion.</t>
   </si>
   <si>
-    <t>HU - 11 Yo como usuario registrado, puedo ver el resumen de mi pedido y/o mandarlo a imprimir.</t>
+    <t>HU - 9 Yo como usuario registrado, quiero finalizar el pedido/compra.</t>
+  </si>
+  <si>
+    <t>HU - 10 Yo como usuario registrado, puedo cambiar mi foto de perfil.</t>
   </si>
 </sst>
 </file>
@@ -586,10 +583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89DF4E1-6287-45C0-B5CD-106EE4FEB071}">
-  <dimension ref="A3:A25"/>
+  <dimension ref="A3:A24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +606,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -624,12 +621,12 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -644,27 +641,22 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>